<commit_message>
Second version. Added image save, image in excel and alt text
</commit_message>
<xml_diff>
--- a/excel-barcode-url-fetcher/data/test_data.xlsx
+++ b/excel-barcode-url-fetcher/data/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\scripts\excel-barcode-url-fetcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\scripts\excel-barcode-url-fetcher\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98355FF9-E7CE-4A72-BD21-9AF81BBCCE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E18035-E244-409B-8839-EC788E847970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="735" windowWidth="13935" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -381,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3053D3-7E4B-4FFE-9564-4A0D459FEBA0}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -424,71 +424,6 @@
         <v>4600999011504</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4751023292441</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4600999010842</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>4600999010828</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>4600999010804</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>4600999011337</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>4607068629714</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>4607068627291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>4607068621817</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>4607068621824</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>4870007340562</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>4870007340593</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>4640130799090</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>4640130799076</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>